<commit_message>
update path to file for print
</commit_message>
<xml_diff>
--- a/src/main/resources/by/bobruisk/zhelnov/myproject/mavenproject1/Original.xlsx
+++ b/src/main/resources/by/bobruisk/zhelnov/myproject/mavenproject1/Original.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="6675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="6675" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="6" r:id="rId1"/>
@@ -18,15 +13,15 @@
   </sheets>
   <definedNames>
     <definedName name="_GoBack" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$M$57</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Лист3!$A$1:$Q$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Лист1'!$A$1:$M$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Лист3'!$A$1:$Q$38</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="287">
   <si>
     <t>Эритроциты</t>
   </si>
@@ -72,7 +67,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -125,7 +120,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
@@ -176,7 +171,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -478,7 +473,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -551,7 +546,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -637,7 +632,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -653,7 +648,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -674,7 +669,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -690,7 +685,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -706,7 +701,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -727,7 +722,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -743,7 +738,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -764,7 +759,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -785,7 +780,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -1109,7 +1104,7 @@
     </r>
     <r>
       <rPr>
-        <u/>
+        <u val="single"/>
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -1135,7 +1130,7 @@
     <t xml:space="preserve">Приложение 10 </t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>УЗ Бобруйска городская поликлиника № 100</t>
@@ -1144,22 +1139,25 @@
     <t>2000</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>Лыко</t>
-  </si>
-  <si>
-    <t>Мама</t>
-  </si>
-  <si>
-    <t>Папа</t>
-  </si>
-  <si>
-    <t>Бабушка</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Лынькова</t>
+  </si>
+  <si>
+    <t>Желнов</t>
+  </si>
+  <si>
+    <t>Антон</t>
+  </si>
+  <si>
+    <t>Олегович</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1171,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="00&quot;.&quot;00&quot;.20&quot;00&quot; &quot;00&quot;:&quot;00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1194,7 +1192,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1208,7 +1206,7 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1230,7 +1228,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1275,7 +1273,7 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1305,17 +1303,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1336,393 +1327,425 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <top style="thin"/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="10" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Comma" xfId="4"/>
-    <cellStyle name="Comma [0]" xfId="5"/>
-    <cellStyle name="Currency" xfId="2"/>
-    <cellStyle name="Currency [0]" xfId="3"/>
-    <cellStyle name="Normal" xfId="6"/>
-    <cellStyle name="Percent" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0"/>
+    <cellStyle name="Percent" xfId="15"/>
+    <cellStyle name="Currency" xfId="16"/>
+    <cellStyle name="Currency [0]" xfId="17"/>
+    <cellStyle name="Comma" xfId="18"/>
+    <cellStyle name="Comma [0]" xfId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
@@ -1998,25 +2021,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleSheetLayoutView="130" workbookViewId="0" topLeftCell="A34">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="3.57421875" style="10" customWidth="1" collapsed="1"/>
     <col min="2" max="6" width="9.140625" style="10" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="1.28515625" style="10" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="3.140625" style="10" customWidth="1" collapsed="1"/>
     <col min="9" max="10" width="9.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.5703125" style="10" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.28125" style="10" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="6.57421875" style="10" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="10.140625" style="10" customWidth="1" collapsed="1"/>
     <col min="14" max="20" width="9.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="9.140625" style="10" collapsed="1"/>
+    <col min="21" max="16384" width="9.140625" style="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="12.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>278</v>
       </c>
@@ -2040,7 +2063,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="12.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -2059,7 +2082,7 @@
       </c>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="12.75" customHeight="1">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -2078,7 +2101,7 @@
       </c>
       <c r="M3" s="27"/>
     </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="12.75" customHeight="1">
       <c r="A4" s="25"/>
       <c r="B4" s="25" t="s">
         <v>249</v>
@@ -2096,7 +2119,7 @@
       <c r="L4" s="25"/>
       <c r="M4" s="25"/>
     </row>
-    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="12.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>255</v>
       </c>
@@ -2121,10 +2144,10 @@
       </c>
       <c r="M5" s="25"/>
     </row>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="12.75" customHeight="1">
       <c r="A6" s="25" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  Мама Папа Бабушка</v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -2134,7 +2157,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  Мама Папа Бабушка</v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -2142,10 +2165,10 @@
       <c r="L6" s="25"/>
       <c r="M6" s="25"/>
     </row>
-    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="12.75" customHeight="1">
       <c r="A7" s="25" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",D56,".",E56,".",F56)</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000</v>
+        <v>2. Число, месяц, год рождения: 3.2.2000</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -2155,7 +2178,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="25" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",D56,".",E56,".",F56)</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000</v>
+        <v>2. Число, месяц, год рождения: 3.2.2000</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
@@ -2163,7 +2186,7 @@
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="12.75" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>247</v>
       </c>
@@ -2182,10 +2205,10 @@
       <c r="L8" s="25"/>
       <c r="M8" s="25"/>
     </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="12.75" customHeight="1">
       <c r="A9" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("4. Адрес: ",C57,", дом ",E57),IF(F57="",CONCATENATE("4. Адрес: ",C57,", дом ",E57,F57,", квартира ",G57),CONCATENATE("4. Адрес:  ",C57,", дом ",E57,", корпус ",F57,", квартира ",G57)))</f>
-        <v>4. Адрес: Лыко, дом 45</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -2195,7 +2218,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("4. Адрес: ",C57,", дом ",E57),IF(F57="",CONCATENATE("4. Адрес: ",C57,", дом ",E57,F57,", квартира ",G57),CONCATENATE("4. Адрес:  ",C57,", дом ",E57,", корпус ",F57,", квартира ",G57)))</f>
-        <v>4. Адрес: Лыко, дом 45</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
@@ -2203,7 +2226,7 @@
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
     </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="12.75" customHeight="1">
       <c r="A10" s="25" t="str">
         <f>CONCATENATE("5. Диагноз: ",TEXT(K54,0),)</f>
         <v>5. Диагноз: Обследование</v>
@@ -2229,7 +2252,7 @@
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
     </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="12.75" customHeight="1">
       <c r="A11" s="25" t="s">
         <v>246</v>
       </c>
@@ -2248,7 +2271,7 @@
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
     </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="12.75" customHeight="1">
       <c r="A12" s="30" t="s">
         <v>194</v>
       </c>
@@ -2279,7 +2302,7 @@
       </c>
       <c r="M12" s="51"/>
     </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="12.75" customHeight="1">
       <c r="A13" s="31">
         <v>1</v>
       </c>
@@ -2306,7 +2329,7 @@
       <c r="L13" s="44"/>
       <c r="M13" s="44"/>
     </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="12.75" customHeight="1">
       <c r="A14" s="31">
         <v>2</v>
       </c>
@@ -2333,7 +2356,7 @@
       <c r="L14" s="44"/>
       <c r="M14" s="44"/>
     </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="12.75" customHeight="1">
       <c r="A15" s="31">
         <v>3</v>
       </c>
@@ -2360,7 +2383,7 @@
       <c r="L15" s="44"/>
       <c r="M15" s="44"/>
     </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="12.75" customHeight="1">
       <c r="A16" s="31">
         <v>4</v>
       </c>
@@ -2387,7 +2410,7 @@
       <c r="L16" s="44"/>
       <c r="M16" s="44"/>
     </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="12.75" customHeight="1">
       <c r="A17" s="31">
         <v>5</v>
       </c>
@@ -2414,7 +2437,7 @@
       <c r="L17" s="44"/>
       <c r="M17" s="44"/>
     </row>
-    <row r="18" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="12.75" customHeight="1">
       <c r="A18" s="31">
         <v>6</v>
       </c>
@@ -2441,7 +2464,7 @@
       <c r="L18" s="44"/>
       <c r="M18" s="44"/>
     </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="12.75" customHeight="1">
       <c r="A19" s="31">
         <v>7</v>
       </c>
@@ -2468,7 +2491,7 @@
       <c r="L19" s="44"/>
       <c r="M19" s="44"/>
     </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="12.75" customHeight="1">
       <c r="A20" s="31">
         <v>8</v>
       </c>
@@ -2495,7 +2518,7 @@
       <c r="L20" s="44"/>
       <c r="M20" s="44"/>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1">
       <c r="A21" s="31">
         <v>9</v>
       </c>
@@ -2520,7 +2543,7 @@
       <c r="L21" s="44"/>
       <c r="M21" s="44"/>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1">
       <c r="A22" s="31"/>
       <c r="B22" s="52" t="s">
         <v>219</v>
@@ -2545,7 +2568,7 @@
       <c r="L22" s="44"/>
       <c r="M22" s="44"/>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1">
       <c r="A23" s="31"/>
       <c r="B23" s="52" t="s">
         <v>216</v>
@@ -2570,7 +2593,7 @@
       <c r="L23" s="44"/>
       <c r="M23" s="44"/>
     </row>
-    <row r="24" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="12.75" customHeight="1">
       <c r="A24" s="31"/>
       <c r="B24" s="52" t="s">
         <v>214</v>
@@ -2595,7 +2618,7 @@
       <c r="L24" s="44"/>
       <c r="M24" s="44"/>
     </row>
-    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="12.75" customHeight="1">
       <c r="A25" s="31"/>
       <c r="B25" s="52" t="s">
         <v>212</v>
@@ -2620,7 +2643,7 @@
       <c r="L25" s="44"/>
       <c r="M25" s="44"/>
     </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="12.75" customHeight="1">
       <c r="A26" s="31"/>
       <c r="B26" s="52" t="s">
         <v>209</v>
@@ -2645,7 +2668,7 @@
       <c r="L26" s="44"/>
       <c r="M26" s="44"/>
     </row>
-    <row r="27" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="12.75" customHeight="1">
       <c r="A27" s="31">
         <v>10</v>
       </c>
@@ -2672,7 +2695,7 @@
       <c r="L27" s="44"/>
       <c r="M27" s="44"/>
     </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="12.75" customHeight="1">
       <c r="A28" s="31">
         <v>11</v>
       </c>
@@ -2699,7 +2722,7 @@
       <c r="L28" s="44"/>
       <c r="M28" s="44"/>
     </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="12.75" customHeight="1">
       <c r="A29" s="31">
         <v>12</v>
       </c>
@@ -2726,7 +2749,7 @@
       <c r="L29" s="44"/>
       <c r="M29" s="44"/>
     </row>
-    <row r="30" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="12.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>199</v>
       </c>
@@ -2745,7 +2768,7 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
     </row>
-    <row r="31" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="12.75" customHeight="1">
       <c r="A31" s="25" t="s">
         <v>198</v>
       </c>
@@ -2764,7 +2787,7 @@
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
     </row>
-    <row r="32" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="12.75" customHeight="1">
       <c r="A32" s="25" t="s">
         <v>197</v>
       </c>
@@ -2783,7 +2806,7 @@
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
     </row>
-    <row r="33" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="12.75" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>196</v>
       </c>
@@ -2798,7 +2821,7 @@
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
     </row>
-    <row r="34" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:12" ht="12.75" customHeight="1">
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -2806,7 +2829,7 @@
       <c r="K34" s="25"/>
       <c r="L34" s="25"/>
     </row>
-    <row r="35" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="12.75" customHeight="1">
       <c r="A35" s="1" t="str">
         <f>A1</f>
         <v>УЗ Бобруйска городская поликлиника № 100</v>
@@ -2821,7 +2844,7 @@
       <c r="K35" s="25"/>
       <c r="L35" s="25"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -2835,7 +2858,7 @@
       <c r="K36" s="25"/>
       <c r="L36" s="25"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -2847,7 +2870,7 @@
       <c r="K37" s="25"/>
       <c r="L37" s="25"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -2862,48 +2885,48 @@
       <c r="K38" s="25"/>
       <c r="L38" s="25"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15">
       <c r="A39" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О: "," ",C55," ",E55," ",F55," ")</f>
-        <v>1. Ф.И.О:  Мама Папа Бабушка</v>
+        <v>1. Ф.И.О:  Желнов Антон Олегович </v>
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" ht="15">
       <c r="A40" s="2" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",D56,".",E56,".",F56,"        3. Пол: мужской, женский(нужное подчеркнуть)")</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000        3. Пол: мужской, женский(нужное подчеркнуть)</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2. Число, месяц, год рождения: 3.2.2000        3. Пол: мужской, женский(нужное подчеркнуть)</v>
+      </c>
+    </row>
+    <row r="41" ht="15">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" ht="15">
       <c r="A42" s="25" t="str">
         <f>IF(VALUE(G57)=0,CONCATENATE("проспект/улица/ переулок/проезд ",C57,", дом ",E57),IF(F57="",CONCATENATE("проспект/улица/ переулок/проезд ",C57," дом ",E57,F57," квартира ",G57),CONCATENATE("Адрес: улица ",C57," дом ",E57," корпус ",F57," квартира ",G57)))</f>
-        <v>проспект/улица/ переулок/проезд Лыко, дом 45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>проспект/улица/ переулок/проезд Лынькова дом 75 квартира 103</v>
+      </c>
+    </row>
+    <row r="43" ht="15">
       <c r="A43" s="2" t="str">
         <f>CONCATENATE("5. Диагноз: ",TEXT(K54,0),)</f>
         <v>5. Диагноз: Обследование</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" ht="15">
       <c r="A44" s="4" t="str">
         <f>CONCATENATE("6. Направил: ",C54," ",F54)</f>
         <v>6. Направил: !Помощник врача! Антон Желнов</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" ht="15">
       <c r="A45" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="33" customHeight="1">
       <c r="A46" s="8" t="s">
         <v>194</v>
       </c>
@@ -2922,7 +2945,7 @@
       <c r="H46" s="39"/>
       <c r="I46" s="39"/>
     </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15" customHeight="1">
       <c r="A47" s="8">
         <v>1</v>
       </c>
@@ -2939,7 +2962,7 @@
       <c r="H47" s="41"/>
       <c r="I47" s="41"/>
     </row>
-    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="15" customHeight="1">
       <c r="A48" s="8">
         <v>2</v>
       </c>
@@ -2956,22 +2979,22 @@
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" ht="15">
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" ht="15">
       <c r="A50" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" ht="15">
       <c r="A51" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:13" ht="15">
       <c r="C53" s="7" t="s">
         <v>25</v>
       </c>
@@ -2992,7 +3015,7 @@
       <c r="L53" s="55"/>
       <c r="M53" s="55"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:13" ht="15">
       <c r="C54" s="6" t="s">
         <v>27</v>
       </c>
@@ -3008,7 +3031,7 @@
       <c r="L54" s="53"/>
       <c r="M54" s="38"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="15">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>
@@ -3034,14 +3057,14 @@
       </c>
       <c r="M55" s="56"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="29" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="E56" s="28" t="s">
         <v>277</v>
@@ -3053,7 +3076,7 @@
       <c r="H56" s="32"/>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="8" t="s">
         <v>29</v>
       </c>
@@ -3166,28 +3189,29 @@
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
   </mergeCells>
-  <pageMargins left="0.196850393700787" right="0.118110236220472" top="0.15748031496063" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins left="0.196850393700787" right="0.118110236220472" top="0.15748031496063" bottom="0.748031496062992" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="portrait" paperSize="9" scale="99" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O93"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0" topLeftCell="A1">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" style="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.421875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.00390625" style="10" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="9.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="10" max="16384" width="9.140625" style="10" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="11.85" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>273</v>
       </c>
@@ -3202,7 +3226,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="11.85" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3218,13 +3242,13 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="11.85" customHeight="1">
       <c r="A3" s="1"/>
       <c r="I3" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="11.85" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -3239,7 +3263,7 @@
       <c r="N4" s="58"/>
       <c r="O4" s="58"/>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3255,38 +3279,38 @@
         <v>Отделение ООВП №2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="11.85" customHeight="1">
       <c r="A6" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: Мама Папа Бабушка</v>
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
       </c>
       <c r="H6" s="2" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: Мама Папа Бабушка</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="11.85" customHeight="1">
       <c r="A7" s="2" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",Лист1!D56,".",Лист1!E56,".",Лист1!F56)</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000</v>
+        <v>2. Число, месяц, год рождения: 3.2.2000</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="2" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",Лист1!D56,".",Лист1!E56,".",Лист1!F56)</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2. Число, месяц, год рождения: 3.2.2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="11.85" customHeight="1">
       <c r="A8" s="2" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: Лыко, дом 45</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="H8" s="2" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: Лыко, дом 45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="11.85" customHeight="1">
       <c r="A9" s="2" t="str">
         <f>CONCATENATE("5. Диагноз: ",TEXT(Лист1!K54,0))</f>
         <v>5. Диагноз: Обследование</v>
@@ -3296,7 +3320,7 @@
         <v>5. Диагноз: Обследование</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="11.85" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -3304,7 +3328,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="11.85" customHeight="1">
       <c r="A11" s="57" t="s">
         <v>34</v>
       </c>
@@ -3317,7 +3341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="11.85" customHeight="1">
       <c r="A12" s="13">
         <v>1</v>
       </c>
@@ -3345,7 +3369,7 @@
       </c>
       <c r="N12" s="72"/>
     </row>
-    <row r="13" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="11.85" customHeight="1">
       <c r="A13" s="13">
         <v>2</v>
       </c>
@@ -3369,7 +3393,7 @@
       <c r="M13" s="68"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="11.85" customHeight="1">
       <c r="A14" s="13">
         <v>3</v>
       </c>
@@ -3395,7 +3419,7 @@
       <c r="M14" s="79"/>
       <c r="N14" s="81"/>
     </row>
-    <row r="15" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="11.85" customHeight="1">
       <c r="A15" s="13">
         <v>4</v>
       </c>
@@ -3417,7 +3441,7 @@
       <c r="M15" s="82"/>
       <c r="N15" s="84"/>
     </row>
-    <row r="16" spans="1:15" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="11.85" customHeight="1">
       <c r="A16" s="13">
         <v>5</v>
       </c>
@@ -3441,7 +3465,7 @@
       <c r="M16" s="68"/>
       <c r="N16" s="69"/>
     </row>
-    <row r="17" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="11.85" customHeight="1">
       <c r="A17" s="13">
         <v>6</v>
       </c>
@@ -3467,7 +3491,7 @@
       <c r="M17" s="79"/>
       <c r="N17" s="81"/>
     </row>
-    <row r="18" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="11.85" customHeight="1">
       <c r="A18" s="13">
         <v>7</v>
       </c>
@@ -3489,7 +3513,7 @@
       <c r="M18" s="82"/>
       <c r="N18" s="84"/>
     </row>
-    <row r="19" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="11.85" customHeight="1">
       <c r="A19" s="13">
         <v>8</v>
       </c>
@@ -3511,7 +3535,7 @@
       <c r="M19" s="68"/>
       <c r="N19" s="69"/>
     </row>
-    <row r="20" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="11.85" customHeight="1">
       <c r="A20" s="13">
         <v>9</v>
       </c>
@@ -3537,7 +3561,7 @@
       <c r="M20" s="79"/>
       <c r="N20" s="81"/>
     </row>
-    <row r="21" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="11.85" customHeight="1">
       <c r="A21" s="13">
         <v>10</v>
       </c>
@@ -3559,7 +3583,7 @@
       <c r="M21" s="82"/>
       <c r="N21" s="84"/>
     </row>
-    <row r="22" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="11.85" customHeight="1">
       <c r="A22" s="13">
         <v>11</v>
       </c>
@@ -3583,7 +3607,7 @@
       <c r="M22" s="68"/>
       <c r="N22" s="69"/>
     </row>
-    <row r="23" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="11.85" customHeight="1">
       <c r="A23" s="13">
         <v>12</v>
       </c>
@@ -3609,7 +3633,7 @@
       <c r="M23" s="79"/>
       <c r="N23" s="81"/>
     </row>
-    <row r="24" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="11.85" customHeight="1">
       <c r="A24" s="13">
         <v>13</v>
       </c>
@@ -3631,7 +3655,7 @@
       <c r="M24" s="82"/>
       <c r="N24" s="84"/>
     </row>
-    <row r="25" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="11.85" customHeight="1">
       <c r="A25" s="13">
         <v>14</v>
       </c>
@@ -3653,7 +3677,7 @@
       <c r="M25" s="68"/>
       <c r="N25" s="69"/>
     </row>
-    <row r="26" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="11.85" customHeight="1">
       <c r="A26" s="13">
         <v>15</v>
       </c>
@@ -3679,7 +3703,7 @@
       <c r="M26" s="79"/>
       <c r="N26" s="81"/>
     </row>
-    <row r="27" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="11.85" customHeight="1">
       <c r="A27" s="13">
         <v>16</v>
       </c>
@@ -3701,7 +3725,7 @@
       <c r="M27" s="82"/>
       <c r="N27" s="84"/>
     </row>
-    <row r="28" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="11.85" customHeight="1">
       <c r="A28" s="13">
         <v>17</v>
       </c>
@@ -3723,7 +3747,7 @@
       <c r="M28" s="68"/>
       <c r="N28" s="69"/>
     </row>
-    <row r="29" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="11.85" customHeight="1">
       <c r="A29" s="13">
         <v>18</v>
       </c>
@@ -3749,7 +3773,7 @@
       <c r="M29" s="79"/>
       <c r="N29" s="81"/>
     </row>
-    <row r="30" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="11.85" customHeight="1">
       <c r="A30" s="13">
         <v>19</v>
       </c>
@@ -3771,7 +3795,7 @@
       <c r="M30" s="82"/>
       <c r="N30" s="84"/>
     </row>
-    <row r="31" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="11.85" customHeight="1">
       <c r="A31" s="13">
         <v>20</v>
       </c>
@@ -3793,7 +3817,7 @@
       <c r="M31" s="68"/>
       <c r="N31" s="69"/>
     </row>
-    <row r="32" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="11.85" customHeight="1">
       <c r="A32" s="13">
         <v>21</v>
       </c>
@@ -3819,7 +3843,7 @@
       <c r="M32" s="79"/>
       <c r="N32" s="81"/>
     </row>
-    <row r="33" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="11.85" customHeight="1">
       <c r="A33" s="13">
         <v>22</v>
       </c>
@@ -3841,7 +3865,7 @@
       <c r="M33" s="82"/>
       <c r="N33" s="84"/>
     </row>
-    <row r="34" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="11.85" customHeight="1">
       <c r="A34" s="13">
         <v>23</v>
       </c>
@@ -3863,7 +3887,7 @@
       <c r="M34" s="68"/>
       <c r="N34" s="69"/>
     </row>
-    <row r="35" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="11.85" customHeight="1">
       <c r="A35" s="13">
         <v>24</v>
       </c>
@@ -3889,7 +3913,7 @@
       <c r="M35" s="79"/>
       <c r="N35" s="81"/>
     </row>
-    <row r="36" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="11.85" customHeight="1">
       <c r="A36" s="13">
         <v>25</v>
       </c>
@@ -3911,7 +3935,7 @@
       <c r="M36" s="82"/>
       <c r="N36" s="84"/>
     </row>
-    <row r="37" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="11.85" customHeight="1">
       <c r="A37" s="13">
         <v>26</v>
       </c>
@@ -3933,7 +3957,7 @@
       <c r="M37" s="59"/>
       <c r="N37" s="60"/>
     </row>
-    <row r="38" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="11.85" customHeight="1">
       <c r="A38" s="13">
         <v>27</v>
       </c>
@@ -3955,7 +3979,7 @@
       <c r="M38" s="61"/>
       <c r="N38" s="62"/>
     </row>
-    <row r="39" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="11.85" customHeight="1">
       <c r="A39" s="13">
         <v>28</v>
       </c>
@@ -3977,7 +4001,7 @@
       <c r="M39" s="63"/>
       <c r="N39" s="64"/>
     </row>
-    <row r="40" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="11.85" customHeight="1">
       <c r="A40" s="13">
         <v>29</v>
       </c>
@@ -3995,7 +4019,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="11.85" customHeight="1">
       <c r="A41" s="13">
         <v>30</v>
       </c>
@@ -4013,7 +4037,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="11.85" customHeight="1">
       <c r="A42" s="36">
         <v>31</v>
       </c>
@@ -4028,7 +4052,7 @@
       </c>
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="11.85" customHeight="1">
       <c r="A43" s="13">
         <v>32</v>
       </c>
@@ -4047,7 +4071,7 @@
         <v>Направил: !Помощник врача! Антон Желнов</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="11.85" customHeight="1">
       <c r="A44" s="13">
         <v>33</v>
       </c>
@@ -4062,7 +4086,7 @@
       </c>
       <c r="E44" s="13"/>
     </row>
-    <row r="45" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="11.85" customHeight="1">
       <c r="A45" s="13">
         <v>34</v>
       </c>
@@ -4080,7 +4104,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="11.85" customHeight="1">
       <c r="A46" s="13">
         <v>35</v>
       </c>
@@ -4101,12 +4125,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" ht="11.85" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>119</v>
       </c>
@@ -4114,14 +4138,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="11.85" customHeight="1">
       <c r="A49" s="4" t="str">
         <f>CONCATENATE("Направил: ",Лист1!C54," ",Лист1!F54)</f>
         <v>Направил: !Помощник врача! Антон Желнов</v>
       </c>
       <c r="N49" s="17"/>
     </row>
-    <row r="50" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="16.5" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>22</v>
       </c>
@@ -4129,49 +4153,49 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:14" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="11.85" customHeight="1"/>
+    <row r="52" ht="11.85" customHeight="1"/>
+    <row r="53" ht="11.85" customHeight="1"/>
+    <row r="54" ht="11.85" customHeight="1"/>
+    <row r="55" ht="11.85" customHeight="1"/>
+    <row r="56" ht="11.85" customHeight="1"/>
+    <row r="57" ht="11.85" customHeight="1"/>
+    <row r="58" ht="11.85" customHeight="1"/>
+    <row r="59" ht="11.85" customHeight="1"/>
+    <row r="60" ht="11.85" customHeight="1"/>
+    <row r="61" ht="11.85" customHeight="1"/>
+    <row r="62" ht="11.85" customHeight="1"/>
+    <row r="63" ht="11.85" customHeight="1"/>
+    <row r="64" ht="11.85" customHeight="1"/>
+    <row r="65" ht="11.85" customHeight="1"/>
+    <row r="66" ht="11.85" customHeight="1"/>
+    <row r="67" ht="11.85" customHeight="1"/>
+    <row r="68" ht="11.85" customHeight="1"/>
+    <row r="69" ht="11.85" customHeight="1"/>
+    <row r="70" ht="11.85" customHeight="1"/>
+    <row r="71" ht="11.85" customHeight="1"/>
+    <row r="72" ht="11.85" customHeight="1"/>
+    <row r="73" ht="11.85" customHeight="1"/>
+    <row r="74" ht="11.85" customHeight="1"/>
+    <row r="75" ht="11.85" customHeight="1"/>
+    <row r="76" ht="11.85" customHeight="1"/>
+    <row r="77" ht="11.85" customHeight="1"/>
+    <row r="78" ht="11.85" customHeight="1"/>
+    <row r="79" ht="11.85" customHeight="1"/>
+    <row r="80" ht="11.85" customHeight="1"/>
+    <row r="81" ht="11.85" customHeight="1"/>
+    <row r="82" ht="11.85" customHeight="1"/>
+    <row r="83" ht="11.85" customHeight="1"/>
+    <row r="84" ht="11.85" customHeight="1"/>
+    <row r="85" ht="11.85" customHeight="1"/>
+    <row r="86" ht="11.85" customHeight="1"/>
+    <row r="87" ht="11.85" customHeight="1"/>
+    <row r="88" ht="11.85" customHeight="1"/>
+    <row r="89" ht="11.85" customHeight="1"/>
+    <row r="90" ht="11.85" customHeight="1"/>
+    <row r="91" ht="11.85" customHeight="1"/>
+    <row r="92" ht="36.75" customHeight="1"/>
+    <row r="93" ht="24.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="86">
     <mergeCell ref="H35:J35"/>
@@ -4261,8 +4285,9 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="M12:N12"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094499" right="0.23622047244094499" top="0.15748031496063" bottom="0.15748031496063" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="95" fitToWidth="2" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins left="0.236220472440945" right="0.236220472440945" top="0.15748031496063" bottom="0.15748031496063" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup fitToHeight="0" fitToWidth="2" horizontalDpi="600" verticalDpi="600" orientation="landscape" paperSize="9" scale="95" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="50" max="16383" man="1"/>
   </rowBreaks>
@@ -4273,22 +4298,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0" topLeftCell="A1">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="12" width="9.140625" style="18" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="7.140625" style="18" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.28515625" style="18" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.5703125" style="18" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8" style="18" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.28125" style="18" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.57421875" style="18" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.00390625" style="18" customWidth="1" collapsed="1"/>
     <col min="17" max="23" width="9.140625" style="18" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="9.140625" style="18" collapsed="1"/>
+    <col min="24" max="16384" width="9.140625" style="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>273</v>
       </c>
@@ -4299,7 +4324,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="23"/>
       <c r="E2" s="23" t="s">
         <v>174</v>
@@ -4308,12 +4333,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="L3" s="20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="23"/>
       <c r="D4" s="24" t="s">
         <v>149</v>
@@ -4323,7 +4348,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="9:13" ht="15.75" customHeight="1">
       <c r="I5" s="18" t="s">
         <v>256</v>
       </c>
@@ -4333,7 +4358,7 @@
         <v>Отделение ООВП №2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="23" t="s">
         <v>146</v>
       </c>
@@ -4342,7 +4367,7 @@
       </c>
       <c r="M6" s="20"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
@@ -4352,57 +4377,57 @@
       </c>
       <c r="I7" s="18" t="str">
         <f>CONCATENATE("1. Фамилия :  ",Лист1!C55,"                                                            2. Имя:  ",Лист1!E55)</f>
-        <v>1. Фамилия :  Мама                                                            2. Имя:  Папа</v>
+        <v>1. Фамилия :  Желнов                                                            2. Имя:  Антон</v>
       </c>
       <c r="M7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="str">
         <f>CONCATENATE("1. Ф.И.О. пациента: ",Лист1!C55," ",Лист1!E55," ",Лист1!F55," ")</f>
-        <v>1. Ф.И.О. пациента: Мама Папа Бабушка</v>
+        <v>1. Ф.И.О. пациента: Желнов Антон Олегович </v>
       </c>
       <c r="I8" s="18" t="str">
         <f>CONCATENATE("3. Отчество:  ",Лист1!F55,"")</f>
-        <v>3. Отчество:  Бабушка</v>
+        <v>3. Отчество:  Олегович</v>
       </c>
       <c r="L8" s="18" t="str">
         <f>CONCATENATE("4. Число, месяц, год рождения: ",Лист1!D56,".",Лист1!E56,".",Лист1!F56)</f>
-        <v>4. Число, месяц, год рождения: 1.1.2000</v>
+        <v>4. Число, месяц, год рождения: 3.2.2000</v>
       </c>
       <c r="M8" s="20"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="str">
         <f>CONCATENATE("2. Число, месяц, год рождения: ",Лист1!D56,".",Лист1!E56,".",Лист1!F56)</f>
-        <v>2. Число, месяц, год рождения: 1.1.2000</v>
+        <v>2. Число, месяц, год рождения: 3.2.2000</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>144</v>
       </c>
       <c r="M9" s="20"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="21" t="str">
         <f>IF(VALUE(Лист1!G57)=0,CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57),IF(Лист1!F57="",CONCATENATE("4. Адрес: ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("4. Адрес:  ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57)))</f>
-        <v>4. Адрес: Лыко, дом 45</v>
+        <v>4. Адрес: Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>143</v>
       </c>
       <c r="M10" s="20"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="21" t="str">
         <f>CONCATENATE("5. Диагноз: ",TEXT(Лист1!K54,0))</f>
         <v>5. Диагноз: Обследование</v>
       </c>
       <c r="I11" s="18" t="str">
         <f>IF(Лист1!F57="",CONCATENATE("проспект/улица/переулок/проезд ",Лист1!C57,", дом ",Лист1!E57,Лист1!F57,", квартира ",Лист1!G57),CONCATENATE("проспект/улица/переулок/проезд ",Лист1!C57,", дом ",Лист1!E57,", корпус ",Лист1!F57,", квартира ",Лист1!G57))</f>
-        <v>проспект/улица/переулок/проезд Лыко, дом 45, квартира 0</v>
+        <v>проспект/улица/переулок/проезд Лынькова, дом 75, квартира 103</v>
       </c>
       <c r="M11" s="20"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="18" t="str">
         <f>CONCATENATE("6. Направил: ",Лист1!C54," ",Лист1!F54)</f>
         <v>6. Направил: !Помощник врача! Антон Желнов</v>
@@ -4413,7 +4438,7 @@
       </c>
       <c r="M12" s="20"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="21" t="s">
         <v>163</v>
       </c>
@@ -4422,7 +4447,7 @@
       </c>
       <c r="M13" s="20"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>142</v>
       </c>
@@ -4431,7 +4456,7 @@
       </c>
       <c r="M14" s="20"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>141</v>
       </c>
@@ -4440,7 +4465,7 @@
       </c>
       <c r="M15" s="20"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15.75" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>140</v>
       </c>
@@ -4456,7 +4481,7 @@
       <c r="P16" s="91"/>
       <c r="Q16" s="91"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15.75" customHeight="1">
       <c r="A17" s="19" t="str">
         <f>CONCATENATE("материал на исследование: ",Лист1!C54," ",Лист1!F54)</f>
         <v>материал на исследование: !Помощник врача! Антон Желнов</v>
@@ -4475,7 +4500,7 @@
       </c>
       <c r="Q17" s="92"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15.75" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>137</v>
       </c>
@@ -4493,7 +4518,7 @@
       </c>
       <c r="Q18" s="92"/>
     </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15.75" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>162</v>
       </c>
@@ -4509,7 +4534,7 @@
       </c>
       <c r="Q19" s="92"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15.75" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>161</v>
       </c>
@@ -4525,7 +4550,7 @@
       <c r="P20" s="95"/>
       <c r="Q20" s="95"/>
     </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>160</v>
       </c>
@@ -4541,7 +4566,7 @@
       <c r="P21" s="95"/>
       <c r="Q21" s="95"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
         <v>159</v>
       </c>
@@ -4559,7 +4584,7 @@
       <c r="P22" s="95"/>
       <c r="Q22" s="95"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>158</v>
       </c>
@@ -4577,7 +4602,7 @@
       <c r="P23" s="95"/>
       <c r="Q23" s="95"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15.75" customHeight="1">
       <c r="A24" s="19" t="s">
         <v>157</v>
       </c>
@@ -4595,7 +4620,7 @@
       <c r="P24" s="95"/>
       <c r="Q24" s="95"/>
     </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="19" t="s">
         <v>156</v>
       </c>
@@ -4603,7 +4628,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="19" t="s">
         <v>155</v>
       </c>
@@ -4615,7 +4640,7 @@
         <v>!Помощник врача! Антон Желнов</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>154</v>
       </c>
@@ -4623,7 +4648,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>153</v>
       </c>
@@ -4631,7 +4656,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="19" t="s">
         <v>151</v>
       </c>
@@ -4639,7 +4664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>152</v>
       </c>
@@ -4647,7 +4672,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1">
       <c r="A31" s="19" t="s">
         <v>151</v>
       </c>
@@ -4655,7 +4680,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1">
       <c r="A32" s="19" t="s">
         <v>151</v>
       </c>
@@ -4663,7 +4688,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
         <v>172</v>
       </c>
@@ -4671,7 +4696,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
       <c r="A34" s="19" t="s">
         <v>173</v>
       </c>
@@ -4679,7 +4704,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
       <c r="A35" s="19" t="s">
         <v>22</v>
       </c>
@@ -4687,26 +4712,26 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="K36" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="I37" s="18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="I38" s="18" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="42" ht="12.75">
       <c r="A42" s="25"/>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="57" ht="12.75">
       <c r="G57" s="18">
         <v>0</v>
       </c>
@@ -4749,7 +4774,8 @@
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="N19:O19"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094499" right="0.23622047244094499" top="0.15748031496063" bottom="0.15748031496063" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="98" orientation="landscape" r:id="rId1"/>
+  <printOptions/>
+  <pageMargins left="0.236220472440945" right="0.236220472440945" top="0.15748031496063" bottom="0.15748031496063" header="0" footer="0"/>
+  <pageSetup horizontalDpi="600" verticalDpi="600" orientation="landscape" paperSize="9" scale="98" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>